<commit_message>
fsk_distance_measure: update pin and timing docs
</commit_message>
<xml_diff>
--- a/embedded/fsk_distance_measure/DOC/pin分配.xlsx
+++ b/embedded/fsk_distance_measure/DOC/pin分配.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t xml:space="preserve"> 序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -133,6 +133,18 @@
   </si>
   <si>
     <t>PA6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ENRF</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -506,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -547,7 +559,9 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>29</v>
       </c>
@@ -562,109 +576,140 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
       <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="3"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
       <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
fsk_distance_measure: update pinout doc
</commit_message>
<xml_diff>
--- a/embedded/fsk_distance_measure/DOC/pin分配.xlsx
+++ b/embedded/fsk_distance_measure/DOC/pin分配.xlsx
@@ -92,10 +92,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ENRF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PC4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -112,10 +108,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>使能RF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>使能放大器</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -169,6 +161,14 @@
   </si>
   <si>
     <t>串口收uart3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ENRF TIM3_CH1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使能RF，可脉冲供电</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -545,7 +545,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -554,7 +554,7 @@
     <col min="2" max="3" width="13.73046875" style="2" customWidth="1"/>
     <col min="4" max="4" width="29.19921875" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.06640625" style="2"/>
-    <col min="6" max="6" width="14.3984375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.265625" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
@@ -579,97 +579,111 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
       <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
@@ -681,35 +695,41 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
@@ -723,7 +743,9 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
fsk_distance_measure: optimise the power down to 1%
</commit_message>
<xml_diff>
--- a/embedded/fsk_distance_measure/DOC/pin分配.xlsx
+++ b/embedded/fsk_distance_measure/DOC/pin分配.xlsx
@@ -104,10 +104,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ENOP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>使能放大器</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -169,6 +165,10 @@
   </si>
   <si>
     <t>使能RF，可脉冲供电</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ENOP TIM3_CH2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -545,7 +545,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -589,7 +589,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -599,13 +599,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -621,11 +621,11 @@
         <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -639,11 +639,11 @@
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -651,13 +651,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -667,13 +667,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -683,7 +683,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
@@ -699,13 +699,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="3"/>
@@ -715,13 +715,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="3"/>

</xml_diff>